<commit_message>
New Regression Suite changes.
</commit_message>
<xml_diff>
--- a/src/test/resources/ninjaCRM.xlsx
+++ b/src/test/resources/ninjaCRM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{40D3F919-A0A4-4912-97F3-22C010E22A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{75F8FC70-AE53-4EA3-A4C6-FC00241501A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{1CFC7333-53AF-4A88-8DA3-8719991583FB}"/>
   </bookViews>
@@ -15,7 +15,7 @@
     <sheet name="createProduct" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:E13"/>
+  <oleSize ref="A1:E23"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="109">
   <si>
     <t>TC_NO</t>
   </si>
@@ -282,24 +282,9 @@
     <t>rmgy@9999</t>
   </si>
   <si>
-    <t>CC_CampaignWithStatus</t>
-  </si>
-  <si>
-    <t>CC_CampaignWithExpectedClosedate</t>
-  </si>
-  <si>
-    <t>CC_CreateCampaignCompleteTest</t>
-  </si>
-  <si>
     <t>Progress</t>
   </si>
   <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>108</t>
-  </si>
-  <si>
     <t>18</t>
   </si>
   <si>
@@ -309,9 +294,6 @@
     <t>Complete Test</t>
   </si>
   <si>
-    <t>HelloCampaign</t>
-  </si>
-  <si>
     <t>Contractor</t>
   </si>
   <si>
@@ -336,19 +318,40 @@
     <t>Trainer 2</t>
   </si>
   <si>
-    <t>Prime</t>
-  </si>
-  <si>
-    <t>Youtube</t>
-  </si>
-  <si>
-    <t>whatsapp</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
     <t>Select Campaign</t>
+  </si>
+  <si>
+    <t>HiCampaign</t>
+  </si>
+  <si>
+    <t>BB_CampaignWithStatus</t>
+  </si>
+  <si>
+    <t>BB_CampaignWithExpectedClosedate</t>
+  </si>
+  <si>
+    <t>BB_CreateCampaignCompleteTest</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>1Prime</t>
+  </si>
+  <si>
+    <t>1Youtube</t>
+  </si>
+  <si>
+    <t>1whatsapp</t>
   </si>
 </sst>
 </file>
@@ -873,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BF5D996-F835-46B5-86F5-AB52766959FC}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -928,7 +931,7 @@
         <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -937,16 +940,16 @@
         <v>64</v>
       </c>
       <c r="F2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="G2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I2" t="s">
         <v>98</v>
-      </c>
-      <c r="H2" t="s">
-        <v>95</v>
-      </c>
-      <c r="I2" t="s">
-        <v>107</v>
       </c>
       <c r="J2" t="s">
         <v>64</v>
@@ -995,7 +998,7 @@
         <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>78</v>
@@ -1004,19 +1007,19 @@
         <v>64</v>
       </c>
       <c r="F5" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="G5" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="H5" t="s">
+        <v>90</v>
+      </c>
+      <c r="I5" t="s">
         <v>96</v>
       </c>
-      <c r="I5" t="s">
-        <v>102</v>
-      </c>
       <c r="J5" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="K5" t="s">
         <v>64</v>
@@ -1068,31 +1071,31 @@
         <v>74</v>
       </c>
       <c r="C8" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E8" t="s">
         <v>64</v>
       </c>
       <c r="F8" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="G8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H8" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="I8" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>76</v>
       </c>
       <c r="K8" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="L8" t="s">
         <v>64</v>
@@ -1187,7 +1190,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1226,10 +1229,10 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>103</v>
       </c>
       <c r="E2" t="s">
         <v>64</v>
@@ -1263,13 +1266,13 @@
         <v>59</v>
       </c>
       <c r="C5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" t="s">
         <v>85</v>
       </c>
-      <c r="D5" t="s">
-        <v>88</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="F5" t="s">
         <v>64</v>
@@ -1303,13 +1306,13 @@
         <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="D8" t="s">
         <v>62</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F8" t="s">
         <v>64</v>
@@ -1349,19 +1352,19 @@
         <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="D11" t="s">
         <v>61</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="F11" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G11" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="H11" t="s">
         <v>64</v>

</xml_diff>